<commit_message>
exel y 1 variable cambiada
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8580"/>
+    <workbookView windowWidth="13511" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="140">
   <si>
     <t>Arrays</t>
   </si>
@@ -94,108 +94,108 @@
     <t>¿Para qué se utiliza?: Estas palabras son utilizadas para cuando el usuario inicia un juego y una determinada opcion debera adivinar x palabra.</t>
   </si>
   <si>
-    <t>$partida</t>
-  </si>
-  <si>
-    <t>Índice</t>
-  </si>
-  <si>
-    <t>palabraWordix</t>
-  </si>
-  <si>
-    <t>jugador</t>
-  </si>
-  <si>
-    <t>intentos</t>
-  </si>
-  <si>
-    <t>puntaje</t>
-  </si>
-  <si>
-    <t>valentina</t>
-  </si>
-  <si>
-    <t>maria</t>
-  </si>
-  <si>
-    <t>pedro</t>
-  </si>
-  <si>
-    <t>tomas</t>
-  </si>
-  <si>
-    <t>alejandro</t>
-  </si>
-  <si>
-    <t>martin</t>
-  </si>
-  <si>
-    <t>javier</t>
-  </si>
-  <si>
-    <t>emanuel</t>
+    <t>$collecPartida</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "TINTO", "jugador" =&gt; "valentina", "intentos" =&gt; 1, "puntaje" =&gt; 14)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "TINTO", "jugador" =&gt; "valentina", "intentos" =&gt; 6, "puntaje" =&gt; 0)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "PERRO", "jugador" =&gt; "maria", "intentos" =&gt; 4, "puntaje" =&gt; 13)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "ARBOL", "jugador" =&gt; "pedro", "intentos" =&gt; 3, "puntaje" =&gt; 13)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "GATOS", "jugador" =&gt; "tomas", "intentos" =&gt; 6, "puntaje" =&gt; 0)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "MUJER", "jugador" =&gt; "tomas", "intentos" =&gt; 0, "puntaje" =&gt; 0)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "VERDE", "jugador" =&gt; "alejandro", "intentos" =&gt; 3, "puntaje" =&gt; 14)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "MELON", "jugador" =&gt; "martin", "intentos" =&gt; 2, "puntaje" =&gt; 15)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "HUEVO", "jugador" =&gt; "javier", "intentos" =&gt; 5, "puntaje" =&gt; 9)</t>
+  </si>
+  <si>
+    <t>("palabraWordix" =&gt; "GOTAS", "jugador" =&gt; "emanuel", "intentos" =&gt; 2, "puntaje" =&gt; 15)</t>
   </si>
   <si>
     <t xml:space="preserve">Tipo: Indexado (los índices son numéricos), donde almacena arreglos asociativos </t>
   </si>
   <si>
+    <t>Tipos de datos: Almacena valores String e int.</t>
+  </si>
+  <si>
     <t>¿Para qué se utiliza?: Se utiliza para mantener registros de partidas prejugadas en el juego Wordix.</t>
   </si>
   <si>
     <t>$arrayResumen</t>
   </si>
   <si>
-    <t>Clave</t>
-  </si>
-  <si>
-    <t>Valor</t>
+    <t xml:space="preserve">JUGADOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARTIDAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUNTAJE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VICTORIAS </t>
+  </si>
+  <si>
+    <t>INTENTO 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTENTO 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTENTO 3 </t>
+  </si>
+  <si>
+    <t>INTENTO 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTENTO 5 </t>
+  </si>
+  <si>
+    <t>INTENTO 6</t>
+  </si>
+  <si>
+    <t>Tipo: Asociativo</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena valores String e Int.</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?: Se utiliza para compartir información resumida sobre el rendimiento de un jugador.</t>
+  </si>
+  <si>
+    <t>PALABRAWORDIX</t>
+  </si>
+  <si>
+    <t>JUGADOR</t>
+  </si>
+  <si>
+    <t>INTENTOS</t>
+  </si>
+  <si>
+    <t>PUNTAJE</t>
   </si>
   <si>
     <t>""</t>
   </si>
   <si>
-    <t>partidas</t>
-  </si>
-  <si>
-    <t>victorias</t>
-  </si>
-  <si>
-    <t>intento1</t>
-  </si>
-  <si>
-    <t>intento2</t>
-  </si>
-  <si>
-    <t>intento3</t>
-  </si>
-  <si>
-    <t>intento4</t>
-  </si>
-  <si>
-    <t>intento5</t>
-  </si>
-  <si>
-    <t>intento6</t>
-  </si>
-  <si>
-    <t>Tipo: Asociativo</t>
-  </si>
-  <si>
-    <t>Tipos de datos: Almacena valores String e Int.</t>
-  </si>
-  <si>
-    <t>¿Para qué se utiliza?: Se utiliza para compartir información resumida sobre el rendimiento de un jugador.</t>
-  </si>
-  <si>
     <t xml:space="preserve">$a </t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>¿Para qué se utiliza?: Se utiliza para representar un elemento de la colección de partidas del juego.</t>
   </si>
   <si>
@@ -215,6 +215,225 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: Se utiliza para realizar un seguimiento de los índices de las palabras utilizadas y evitar repeticiones.</t>
+  </si>
+  <si>
+    <t>$teclado</t>
+  </si>
+  <si>
+    <t>"A" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>B" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>C" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>D" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>E" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>F" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>G" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>H" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>I" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>J" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>K" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>L" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>M" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>N" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>Ñ" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>O" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>P" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>Q" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>R" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>S" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>T" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>U" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>V" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>W" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>X" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>Y" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>Z" =&gt; ESTADO_LETRA_DISPONIBLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo:  asociativo </t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena valores string.</t>
+  </si>
+  <si>
+    <t>$ordenTeclado</t>
+  </si>
+  <si>
+    <t>"salto"</t>
+  </si>
+  <si>
+    <t>"Q"</t>
+  </si>
+  <si>
+    <t>"w"</t>
+  </si>
+  <si>
+    <t>"E"</t>
+  </si>
+  <si>
+    <t>"R"</t>
+  </si>
+  <si>
+    <t>"T"</t>
+  </si>
+  <si>
+    <t>"Y"</t>
+  </si>
+  <si>
+    <t>"U"</t>
+  </si>
+  <si>
+    <t>"I"</t>
+  </si>
+  <si>
+    <t>"O"</t>
+  </si>
+  <si>
+    <t>"P"</t>
+  </si>
+  <si>
+    <t>"A"</t>
+  </si>
+  <si>
+    <t>"S"</t>
+  </si>
+  <si>
+    <t>"D"</t>
+  </si>
+  <si>
+    <t>"F"</t>
+  </si>
+  <si>
+    <t>"G"</t>
+  </si>
+  <si>
+    <t>"H"</t>
+  </si>
+  <si>
+    <t>"J"</t>
+  </si>
+  <si>
+    <t>"L"</t>
+  </si>
+  <si>
+    <t>"Z"</t>
+  </si>
+  <si>
+    <t>"X"</t>
+  </si>
+  <si>
+    <t>"C"</t>
+  </si>
+  <si>
+    <t>"V"</t>
+  </si>
+  <si>
+    <t>"B"</t>
+  </si>
+  <si>
+    <t>"N"</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?:Ordena las letras como se deberian ver en el teclado</t>
+  </si>
+  <si>
+    <t>$abc</t>
+  </si>
+  <si>
+    <t>"Ñ"</t>
+  </si>
+  <si>
+    <t>"K"</t>
+  </si>
+  <si>
+    <t>"W"</t>
+  </si>
+  <si>
+    <t>"M"</t>
+  </si>
+  <si>
+    <t>Tipo: Multidimensional (los 3 indices tienen un tipo de letra)</t>
+  </si>
+  <si>
+    <t>¿Para qué se utiliza?:Separa las letras en vocales y consonantes, luego separa de la b-m n-z donde se usaran para el puntaje.</t>
+  </si>
+  <si>
+    <t>#Integrantes del Grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanchez, TOMAS. FAI-4494. TUDW. </t>
+  </si>
+  <si>
+    <t>tomas.sanchez2004@est.fi.uncoma.edu.ar. tomisanchezz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinedo, Emanuel. FAI-4871. TUDW </t>
+  </si>
+  <si>
+    <t>emanuel.pinedo@est.fi.uncoma.edu.ar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javier, Castillo. FAI-4936. TUDW </t>
+  </si>
+  <si>
+    <t>javier.castillo@est.fi.uncoma.edu.ar. JaviCast03</t>
+  </si>
+  <si>
+    <t>URL  repos</t>
+  </si>
+  <si>
+    <t>https://github.com/tomisanchezz/TrabajoPracticoFinalip2.git</t>
   </si>
 </sst>
 </file>
@@ -259,15 +478,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <name val="Segoe UI"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -608,7 +827,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -629,35 +848,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFD9D9E3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFD9D9E3"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -782,7 +972,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -794,34 +984,34 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -906,7 +1096,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -916,17 +1106,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1273,21 +1457,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V98"/>
+  <dimension ref="A1:AD88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.8518518518519" customWidth="1"/>
-    <col min="2" max="2" width="14.287037037037" customWidth="1"/>
-    <col min="3" max="3" width="13.4259259259259" customWidth="1"/>
-    <col min="4" max="4" width="13.712962962963" customWidth="1"/>
-    <col min="5" max="5" width="12.8518518518519" customWidth="1"/>
-    <col min="6" max="6" width="12.287037037037" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="2" max="2" width="20.5092592592593" customWidth="1"/>
+    <col min="3" max="3" width="17.8981481481481" customWidth="1"/>
+    <col min="4" max="5" width="17.7777777777778" customWidth="1"/>
+    <col min="6" max="6" width="18.6851851851852" customWidth="1"/>
+    <col min="7" max="7" width="19.9907407407407" customWidth="1"/>
+    <col min="8" max="8" width="20.3888888888889" customWidth="1"/>
+    <col min="9" max="9" width="17.8981481481481" customWidth="1"/>
+    <col min="10" max="10" width="18.4259259259259" customWidth="1"/>
+    <col min="11" max="11" width="17.7685185185185" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1444,554 +1631,930 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2">
+        <v>7</v>
+      </c>
+      <c r="J11" s="2">
+        <v>8</v>
+      </c>
+      <c r="K11" s="2">
+        <v>9</v>
+      </c>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" ht="21" customHeight="1" spans="2:11">
+      <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="7:7">
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="7:7">
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="7:7">
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="7:7">
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="7:7">
-      <c r="G17" s="5"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="7:7">
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="7:7">
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="7:7">
-      <c r="G20" s="5"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="7:7">
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="7:7">
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="7:7">
-      <c r="G23" s="5"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="I40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="2">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2</v>
+      </c>
+      <c r="E50" s="2">
+        <v>3</v>
+      </c>
+      <c r="F50" s="2">
+        <v>4</v>
+      </c>
+      <c r="G50" s="2">
+        <v>5</v>
+      </c>
+      <c r="H50" s="2">
+        <v>6</v>
+      </c>
+      <c r="I50" s="2">
+        <v>7</v>
+      </c>
+      <c r="J50" s="2">
+        <v>8</v>
+      </c>
+      <c r="K50" s="2">
+        <v>9</v>
+      </c>
+      <c r="L50" s="2">
+        <v>10</v>
+      </c>
+      <c r="M50" s="2">
+        <v>11</v>
+      </c>
+      <c r="N50" s="2">
+        <v>12</v>
+      </c>
+      <c r="O50" s="2">
+        <v>13</v>
+      </c>
+      <c r="P50" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>15</v>
+      </c>
+      <c r="R50" s="2">
+        <v>16</v>
+      </c>
+      <c r="S50" s="2">
+        <v>17</v>
+      </c>
+      <c r="T50" s="2">
+        <v>18</v>
+      </c>
+      <c r="U50" s="2">
+        <v>19</v>
+      </c>
+      <c r="V50" s="2">
+        <v>20</v>
+      </c>
+      <c r="W50" s="2">
+        <v>21</v>
+      </c>
+      <c r="X50" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y50" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z50" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA50" s="2">
+        <v>25</v>
+      </c>
+      <c r="AB50" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" ht="17.55" spans="3:7">
-      <c r="C34" s="6" t="s">
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+    </row>
+    <row r="51" ht="26" customHeight="1" spans="1:30">
+      <c r="A51" s="7"/>
+      <c r="B51" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q51" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="R51" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S51" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="T51" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="U51" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="V51" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="W51" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="X51" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y51" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z51" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA51" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB51" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC51" s="5"/>
+      <c r="AD51" s="5"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29">
+      <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="2">
+        <v>0</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2">
+        <v>2</v>
+      </c>
+      <c r="E57" s="2">
+        <v>3</v>
+      </c>
+      <c r="F57" s="2">
+        <v>4</v>
+      </c>
+      <c r="G57" s="2">
+        <v>5</v>
+      </c>
+      <c r="H57" s="2">
+        <v>6</v>
+      </c>
+      <c r="I57" s="2">
+        <v>7</v>
+      </c>
+      <c r="J57" s="2">
+        <v>8</v>
+      </c>
+      <c r="K57" s="2">
+        <v>9</v>
+      </c>
+      <c r="L57" s="2">
+        <v>10</v>
+      </c>
+      <c r="M57" s="2">
+        <v>11</v>
+      </c>
+      <c r="N57" s="2">
+        <v>12</v>
+      </c>
+      <c r="O57" s="2">
+        <v>13</v>
+      </c>
+      <c r="P57" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q57" s="2">
+        <v>15</v>
+      </c>
+      <c r="R57" s="2">
+        <v>16</v>
+      </c>
+      <c r="S57" s="2">
+        <v>17</v>
+      </c>
+      <c r="T57" s="2">
+        <v>18</v>
+      </c>
+      <c r="U57" s="2">
+        <v>19</v>
+      </c>
+      <c r="V57" s="2">
+        <v>20</v>
+      </c>
+      <c r="W57" s="2">
+        <v>21</v>
+      </c>
+      <c r="X57" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y57" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z57" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA57" s="2">
+        <v>25</v>
+      </c>
+      <c r="AB57" s="2">
+        <v>26</v>
+      </c>
+      <c r="AC57" s="2">
         <v>27</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" ht="17.55" spans="3:7">
-      <c r="C35" s="8">
+    </row>
+    <row r="58" spans="2:29">
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" t="s">
+        <v>101</v>
+      </c>
+      <c r="F58" t="s">
+        <v>102</v>
+      </c>
+      <c r="G58" t="s">
+        <v>103</v>
+      </c>
+      <c r="H58" t="s">
+        <v>104</v>
+      </c>
+      <c r="I58" t="s">
+        <v>105</v>
+      </c>
+      <c r="J58" t="s">
+        <v>106</v>
+      </c>
+      <c r="K58" t="s">
+        <v>107</v>
+      </c>
+      <c r="L58" t="s">
+        <v>108</v>
+      </c>
+      <c r="M58" t="s">
+        <v>98</v>
+      </c>
+      <c r="N58" t="s">
+        <v>109</v>
+      </c>
+      <c r="O58" t="s">
+        <v>110</v>
+      </c>
+      <c r="P58" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>112</v>
+      </c>
+      <c r="R58" t="s">
+        <v>113</v>
+      </c>
+      <c r="S58" t="s">
+        <v>114</v>
+      </c>
+      <c r="T58" t="s">
+        <v>115</v>
+      </c>
+      <c r="U58" t="s">
+        <v>116</v>
+      </c>
+      <c r="V58" t="s">
+        <v>98</v>
+      </c>
+      <c r="W58" t="s">
+        <v>117</v>
+      </c>
+      <c r="X58" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" s="2">
         <v>0</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="9">
+      <c r="C65" s="2">
         <v>1</v>
       </c>
-      <c r="G35" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" ht="17.55" spans="3:7">
-      <c r="C36" s="8">
-        <v>1</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="9">
-        <v>6</v>
-      </c>
-      <c r="G36" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" ht="17.55" spans="3:7">
-      <c r="C37" s="8">
+      <c r="D65" s="2">
         <v>2</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F37" s="9">
-        <v>4</v>
-      </c>
-      <c r="G37" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" ht="17.55" spans="3:7">
-      <c r="C38" s="8">
-        <v>3</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="9">
-        <v>3</v>
-      </c>
-      <c r="G38" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" ht="17.55" spans="3:7">
-      <c r="C39" s="8">
-        <v>4</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F39" s="9">
-        <v>6</v>
-      </c>
-      <c r="G39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" ht="17.55" spans="3:7">
-      <c r="C40" s="8">
-        <v>5</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="9">
-        <v>0</v>
-      </c>
-      <c r="G40" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" ht="17.55" spans="3:7">
-      <c r="C41" s="8">
-        <v>6</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" s="9">
-        <v>3</v>
-      </c>
-      <c r="G41" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" ht="17.55" spans="3:7">
-      <c r="C42" s="8">
-        <v>7</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F42" s="9">
-        <v>2</v>
-      </c>
-      <c r="G42" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" ht="17.55" spans="3:7">
-      <c r="C43" s="8">
-        <v>8</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="9">
-        <v>5</v>
-      </c>
-      <c r="G43" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" ht="16.8" spans="3:7">
-      <c r="C44" s="10">
-        <v>9</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F44" s="11">
-        <v>2</v>
-      </c>
-      <c r="G44" s="11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3">
-      <c r="C46" s="4" t="s">
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" t="s">
+        <v>119</v>
+      </c>
+      <c r="D67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" t="s">
+        <v>111</v>
+      </c>
+      <c r="D68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" t="s">
+        <v>112</v>
+      </c>
+      <c r="D69" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4">
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4">
+      <c r="C72" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4">
+      <c r="C73" t="s">
+        <v>115</v>
+      </c>
+      <c r="D73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4">
+      <c r="C74" t="s">
+        <v>126</v>
+      </c>
+      <c r="D74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4">
+      <c r="C75" t="s">
+        <v>116</v>
+      </c>
+      <c r="D75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4">
+      <c r="C76" t="s">
+        <v>128</v>
+      </c>
+      <c r="D76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4">
+      <c r="D77" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4">
+      <c r="D78" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="3:3">
-      <c r="C47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3">
-      <c r="C48" t="s">
+    <row r="80" spans="2:2">
+      <c r="B80" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="3:3">
-      <c r="C49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" ht="17.55" spans="2:4">
-      <c r="B51" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" ht="17.55" spans="3:4">
-      <c r="C52" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" ht="17.55" spans="3:4">
-      <c r="C53" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" ht="17.55" spans="3:4">
-      <c r="C54" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" ht="17.55" spans="3:4">
-      <c r="C55" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" ht="17.55" spans="3:4">
-      <c r="C56" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" ht="17.55" spans="3:4">
-      <c r="C57" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" ht="17.55" spans="3:4">
-      <c r="C58" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" ht="17.55" spans="3:4">
-      <c r="C59" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D59" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" ht="17.55" spans="3:4">
-      <c r="C60" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" ht="16.8" spans="3:4">
-      <c r="C61" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D61" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3">
-      <c r="C63" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3">
-      <c r="C64" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3">
-      <c r="C65" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3">
-      <c r="C66" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" ht="17.55" spans="2:4">
-      <c r="B68" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" ht="17.55" spans="3:4">
-      <c r="C69" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" ht="17.55" spans="3:4">
-      <c r="C70" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="71" ht="17.55" spans="3:4">
-      <c r="C71" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="72" ht="16.8" spans="3:4">
-      <c r="C72" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3">
-      <c r="C74" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3">
-      <c r="C75" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3">
-      <c r="C76" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3">
-      <c r="C77" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" ht="17.55" spans="2:4">
-      <c r="B79" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="80" ht="17.55" spans="3:4">
-      <c r="C80" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="81" ht="17.55" spans="3:4">
-      <c r="C81" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="82" ht="17.55" spans="3:4">
-      <c r="C82" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="83" ht="16.8" spans="3:4">
-      <c r="C83" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3">
-      <c r="C85" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="86" spans="3:3">
-      <c r="C86" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="87" spans="3:3">
-      <c r="C87" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="88" spans="3:3">
-      <c r="C88" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="90" ht="17.55" spans="2:4">
-      <c r="B90" t="s">
-        <v>63</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="91" ht="17.55" spans="3:4">
-      <c r="C91" s="8">
-        <v>0</v>
-      </c>
-      <c r="D91" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" ht="17.55" spans="3:4">
-      <c r="C92" s="8">
-        <v>1</v>
-      </c>
-      <c r="D92" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" ht="17.55" spans="3:4">
-      <c r="C93" s="8">
-        <v>2</v>
-      </c>
-      <c r="D93" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="94" ht="16.8" spans="3:4">
-      <c r="C94" s="10">
-        <v>3</v>
-      </c>
-      <c r="D94" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3">
-      <c r="C95" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3">
-      <c r="C96" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3">
-      <c r="C97" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3">
-      <c r="C98" t="s">
-        <v>66</v>
+    <row r="82" spans="2:2">
+      <c r="B82" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" ht="28.8" spans="1:2">
+      <c r="A85" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" ht="28.8" spans="1:2">
+      <c r="A86" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B86" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" ht="43.2" spans="1:2">
+      <c r="A87" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B87" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>138</v>
+      </c>
+      <c r="B88" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>